<commit_message>
2 mappen aangemaakt config.php en MySqlDatabaseClass aangemaakt
</commit_message>
<xml_diff>
--- a/Documenten/logboek game.xlsx
+++ b/Documenten/logboek game.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2445" windowWidth="25020" windowHeight="7905" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="25020" windowHeight="11130" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="weeknr 47" sheetId="1" r:id="rId1"/>
@@ -12,11 +12,12 @@
     <sheet name="Totaal" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="144525"/>
+  <oleSize ref="A1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="23">
   <si>
     <t>Logboek</t>
   </si>
@@ -76,6 +77,15 @@
   </si>
   <si>
     <t>Donderdag</t>
+  </si>
+  <si>
+    <t>bug fix connect_db</t>
+  </si>
+  <si>
+    <t>Login tabel gemaakt database. User tabel gemaakt database.</t>
+  </si>
+  <si>
+    <t>config map aangemaakt. Classes map aangemaakt. Config.php gemaakt en de eerste classen aan begonnen</t>
   </si>
 </sst>
 </file>
@@ -807,7 +817,7 @@
   <dimension ref="A1:H26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="F18" sqref="F16:F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -898,44 +908,60 @@
       <c r="C7" s="9">
         <v>0.61805555555555558</v>
       </c>
-      <c r="D7" s="9"/>
+      <c r="D7" s="9">
+        <v>0.63541666666666663</v>
+      </c>
       <c r="E7" s="8">
         <v>1</v>
       </c>
-      <c r="F7" s="12"/>
+      <c r="F7" s="12" t="s">
+        <v>20</v>
+      </c>
       <c r="G7" s="9">
         <f>D7-C7</f>
-        <v>-0.61805555555555558</v>
+        <v>1.7361111111111049E-2</v>
       </c>
       <c r="H7" s="3"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="3"/>
       <c r="B8" s="3"/>
-      <c r="C8" s="9"/>
-      <c r="D8" s="9"/>
+      <c r="C8" s="9">
+        <v>0.63541666666666663</v>
+      </c>
+      <c r="D8" s="9">
+        <v>0.64861111111111114</v>
+      </c>
       <c r="E8" s="8">
         <v>2</v>
       </c>
-      <c r="F8" s="12"/>
+      <c r="F8" s="12" t="s">
+        <v>21</v>
+      </c>
       <c r="G8" s="9">
         <f t="shared" ref="G8:G18" si="0">D8-C8</f>
-        <v>0</v>
+        <v>1.3194444444444509E-2</v>
       </c>
       <c r="H8" s="3"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A9" s="3"/>
       <c r="B9" s="3"/>
-      <c r="C9" s="9"/>
-      <c r="D9" s="9"/>
+      <c r="C9" s="9">
+        <v>0.64930555555555558</v>
+      </c>
+      <c r="D9" s="9">
+        <v>0.66666666666666663</v>
+      </c>
       <c r="E9" s="8">
         <v>3</v>
       </c>
-      <c r="F9" s="12"/>
+      <c r="F9" s="12" t="s">
+        <v>22</v>
+      </c>
       <c r="G9" s="9">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1.7361111111111049E-2</v>
       </c>
       <c r="H9" s="3"/>
     </row>
@@ -1135,7 +1161,7 @@
       </c>
       <c r="G26" s="9">
         <f>SUM(G7:G22)</f>
-        <v>-0.61805555555555558</v>
+        <v>4.7916666666666607E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>